<commit_message>
1. Map Checkitem and CheckitemStatus. 2. Create CheckitemDAO. 3. Test mapping entity and dao. 4. Record wrok time.
</commit_message>
<xml_diff>
--- a/work-record/work-record(Liu).xlsx
+++ b/work-record/work-record(Liu).xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/washizaki/Documents/workspace/java/Checklist/work-record/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -285,6 +290,15 @@
   </si>
   <si>
     <t>４０分</t>
+  </si>
+  <si>
+    <t>2016年11月28日</t>
+  </si>
+  <si>
+    <t>マッピング</t>
+  </si>
+  <si>
+    <t>４時間</t>
   </si>
 </sst>
 </file>
@@ -731,7 +745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,19 +753,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="20" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" customHeight="1">
+    <row r="1" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" customHeight="1">
+    <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -779,7 +793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" customHeight="1">
+    <row r="3" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -793,7 +807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26" customHeight="1">
+    <row r="4" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -807,7 +821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" customHeight="1">
+    <row r="5" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -821,7 +835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" customHeight="1">
+    <row r="6" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -835,7 +849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" customHeight="1">
+    <row r="7" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -844,16 +858,22 @@
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solve the transaction problem and record time of work.
</commit_message>
<xml_diff>
--- a/work-record/work-record(Liu).xlsx
+++ b/work-record/work-record(Liu).xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/washizaki/Documents/workspace/java/Checklist/work-record/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
@@ -16,13 +11,13 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -299,6 +294,45 @@
   </si>
   <si>
     <t>４時間</t>
+  </si>
+  <si>
+    <r>
+      <t>2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>年11月30日</t>
+    </r>
+  </si>
+  <si>
+    <t>solve the problem of transaction</t>
+  </si>
+  <si>
+    <r>
+      <t>2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>年12月1日</t>
+    </r>
+  </si>
+  <si>
+    <t>データベースの設計をもう一度考えた。Transactionの問題を解決した。</t>
+  </si>
+  <si>
+    <t>４時間半</t>
   </si>
 </sst>
 </file>
@@ -745,7 +779,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,19 +787,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="20" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="26" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="26" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -793,7 +827,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="26" customHeight="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -807,7 +841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="26" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -821,7 +855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="26" customHeight="1">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -835,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="26" customHeight="1">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -849,7 +883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="26" customHeight="1">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -860,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="26" customHeight="1">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -869,11 +903,38 @@
       </c>
       <c r="D8" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="26" customHeight="1">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26" customHeight="1">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check class and record work.
</commit_message>
<xml_diff>
--- a/work-record/work-record(Liu).xlsx
+++ b/work-record/work-record(Liu).xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Checklist\work-record\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -106,7 +111,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -151,7 +156,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -172,7 +177,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -228,7 +233,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -248,7 +253,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -333,24 +338,48 @@
   </si>
   <si>
     <t>４時間半</t>
+  </si>
+  <si>
+    <t>データベースの設計を直した。様々な設計を更新した。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4時間</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3時間</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>studied dynamic proxy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>strutsの復習</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2時間</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -359,7 +388,7 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="游明朝"/>
-      <charset val="128"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -379,7 +408,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -388,7 +417,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -446,7 +475,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,20 +494,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -779,7 +839,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -787,19 +847,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="26.1" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="20" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" customHeight="1">
+    <row r="1" spans="1:5" ht="26.1" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" customHeight="1">
+    <row r="2" spans="1:5" ht="26.1" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -827,7 +887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" customHeight="1">
+    <row r="3" spans="1:5" ht="26.1" customHeight="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -841,7 +901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26" customHeight="1">
+    <row r="4" spans="1:5" ht="26.1" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -855,7 +915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" customHeight="1">
+    <row r="5" spans="1:5" ht="26.1" customHeight="1">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -869,7 +929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" customHeight="1">
+    <row r="6" spans="1:5" ht="26.1" customHeight="1">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -883,7 +943,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" customHeight="1">
+    <row r="7" spans="1:5" ht="26.1" customHeight="1">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -894,7 +954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26" customHeight="1">
+    <row r="8" spans="1:5" ht="26.1" customHeight="1">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -905,7 +965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="26" customHeight="1">
+    <row r="9" spans="1:5" ht="26.1" customHeight="1">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -916,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="26" customHeight="1">
+    <row r="10" spans="1:5" ht="26.1" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -925,12 +985,45 @@
       </c>
       <c r="D10" s="5" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="26.1" customHeight="1">
+      <c r="A11" s="6">
+        <v>42706</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="26.1" customHeight="1">
+      <c r="A12" s="6">
+        <v>42707</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="26.1" customHeight="1">
+      <c r="A13" s="6">
+        <v>42707</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>